<commit_message>
ipynb file added and changes
</commit_message>
<xml_diff>
--- a/simple_reg_predict_model.xlsx
+++ b/simple_reg_predict_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91798\linear_regression_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53BC76D-7F72-44FB-878E-866802B5A695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC55979F-3C3B-482A-9EA5-EE492E78C888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D874042-DF0E-4914-8BC4-A047444908B3}"/>
   </bookViews>
@@ -276,22 +276,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +662,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,7 +702,7 @@
       <c r="H1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -737,7 +737,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>3170.9653264765366</v>
       </c>
-      <c r="I2" s="12"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -770,7 +770,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>8192.518606825608</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -803,7 +803,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-2121.9281128253206</v>
       </c>
-      <c r="I4" s="12"/>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -836,7 +836,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6403.4916316035669</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -869,7 +869,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>3905.9448496181867</v>
       </c>
-      <c r="I6" s="12"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -902,7 +902,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>6493.7214897927261</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -935,7 +935,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-1051.7252298582025</v>
       </c>
-      <c r="I8" s="12"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -968,7 +968,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>8948.2747701417975</v>
       </c>
-      <c r="I9" s="12"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1001,7 +1001,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-2908.8420289855203</v>
       </c>
-      <c r="I10" s="12"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1034,7 +1034,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-7064.5121084619095</v>
       </c>
-      <c r="I11" s="12"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1067,7 +1067,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-5901.5121084619095</v>
       </c>
-      <c r="I12" s="12"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1100,7 +1100,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6697.7354682873702</v>
       </c>
-      <c r="I13" s="12"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1133,7 +1133,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-3202.5223468910845</v>
       </c>
-      <c r="I14" s="12"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1166,7 +1166,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6951.9690665420057</v>
       </c>
-      <c r="I15" s="12"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1199,7 +1199,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>1020.24405485428</v>
       </c>
-      <c r="I16" s="12"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1232,7 +1232,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>2554.7768583449943</v>
       </c>
-      <c r="I17" s="12"/>
+      <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -1265,7 +1265,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>12304.10677886862</v>
       </c>
-      <c r="I18" s="12"/>
+      <c r="I18" s="16"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -1298,7 +1298,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-3287.6800997350947</v>
       </c>
-      <c r="I19" s="12"/>
+      <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -1331,7 +1331,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-1756.0202586878731</v>
       </c>
-      <c r="I20" s="12"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -1364,7 +1364,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>1558.4162225338805</v>
       </c>
-      <c r="I21" s="12"/>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1397,7 +1397,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-801.03049711702624</v>
       </c>
-      <c r="I22" s="12"/>
+      <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="12"/>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -1436,33 +1436,33 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="6">
         <f>F23/E23</f>
         <v>9202.2335982546356</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="5">
         <f>B23-(E26*A23)</f>
         <v>26049.577715443367</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
@@ -1476,177 +1476,177 @@
       <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="16">
+      <c r="A33" s="12">
         <v>2</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="12">
         <v>43525</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="13">
         <f t="shared" ref="C33:C41" si="3">$E$27+($E$26*A33)</f>
         <v>44454.044911952638</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D33" s="12">
         <f t="shared" ref="D33:D41" si="4">B33-C33</f>
         <v>-929.04491195263836</v>
       </c>
-      <c r="E33" s="15"/>
+      <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="16">
+      <c r="A34" s="12">
         <v>3.9</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="12">
         <v>63218</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="13">
         <f t="shared" si="3"/>
         <v>61938.288748636442</v>
       </c>
-      <c r="D34" s="16">
-        <f t="shared" si="4"/>
+      <c r="D34" s="12">
+        <f>B34-C34</f>
         <v>1279.7112513635584</v>
       </c>
-      <c r="E34" s="15"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="16">
+      <c r="A35" s="12">
         <v>4.5</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="12">
         <v>61111</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="13">
         <f t="shared" si="3"/>
         <v>67459.628907589227</v>
       </c>
-      <c r="D35" s="16">
+      <c r="D35" s="12">
         <f t="shared" si="4"/>
         <v>-6348.6289075892273</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="17"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="16">
+      <c r="A36" s="12">
         <v>5.3</v>
       </c>
-      <c r="B36" s="16">
+      <c r="B36" s="12">
         <v>83088</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="13">
         <f t="shared" si="3"/>
         <v>74821.415786192927</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D36" s="12">
         <f t="shared" si="4"/>
         <v>8266.584213807073</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="17"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="16">
+      <c r="A37" s="12">
         <v>6</v>
       </c>
-      <c r="B37" s="16">
+      <c r="B37" s="12">
         <v>93940</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="13">
         <f t="shared" si="3"/>
         <v>81262.979304971173</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D37" s="12">
         <f t="shared" si="4"/>
         <v>12677.020695028827</v>
       </c>
-      <c r="E37" s="15"/>
+      <c r="E37" s="17"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="16">
+      <c r="A38" s="12">
         <v>6.8</v>
       </c>
-      <c r="B38" s="16">
+      <c r="B38" s="12">
         <v>91738</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="13">
         <f t="shared" si="3"/>
         <v>88624.766183574888</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D38" s="12">
         <f t="shared" si="4"/>
         <v>3113.2338164251123</v>
       </c>
-      <c r="E38" s="15"/>
+      <c r="E38" s="17"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="16">
+      <c r="A39" s="12">
         <v>7.1</v>
       </c>
-      <c r="B39" s="16">
+      <c r="B39" s="12">
         <v>98273</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="13">
         <f t="shared" si="3"/>
         <v>91385.436263051277</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="12">
         <f t="shared" si="4"/>
         <v>6887.5637369487231</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="17"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="16">
+      <c r="A40" s="12">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B40" s="16">
+      <c r="B40" s="12">
         <v>109431</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="13">
         <f t="shared" si="3"/>
         <v>106109.01002025869</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D40" s="12">
         <f t="shared" si="4"/>
         <v>3321.9899797413091</v>
       </c>
-      <c r="E40" s="15"/>
+      <c r="E40" s="17"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="16">
+      <c r="A41" s="12">
         <v>9.5</v>
       </c>
-      <c r="B41" s="16">
+      <c r="B41" s="12">
         <v>116969</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="13">
         <f t="shared" si="3"/>
         <v>113470.79689886241</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D41" s="12">
         <f t="shared" si="4"/>
         <v>3498.2031011375948</v>
       </c>
-      <c r="E41" s="15"/>
+      <c r="E41" s="17"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="14" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some points like MAPE,RSS,TSS,MSE
</commit_message>
<xml_diff>
--- a/simple_reg_predict_model.xlsx
+++ b/simple_reg_predict_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91798\linear_regression_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC55979F-3C3B-482A-9EA5-EE492E78C888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D93CAA-5501-4615-8BCB-D8FAEAC46A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D874042-DF0E-4914-8BC4-A047444908B3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>x</t>
   </si>
@@ -98,9 +98,6 @@
     <t xml:space="preserve">  y - ŷ</t>
   </si>
   <si>
-    <t>Randomly 30% of the data</t>
-  </si>
-  <si>
     <t>Randomly 70% of the data</t>
   </si>
   <si>
@@ -114,6 +111,72 @@
   </si>
   <si>
     <t xml:space="preserve"> ŷ  =  26049.5777  +  ( 9202.2335 * x )</t>
+  </si>
+  <si>
+    <t>RSS = (y - ŷ)^2</t>
+  </si>
+  <si>
+    <t>TSS = ( y - y̅ )^2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total Observation = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <t>R Square Value                   R^2 = 1 - (RSS/TSS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mean Square Error                     MSE = RSS / N </t>
+  </si>
+  <si>
+    <t>y̅</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Root Mean Square Error           RMSE  =  sqrt(MSE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mean Absolute Percentage Error    MAPE  =  M / N</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> M = ( |y - ŷ| ) / y   =   |</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>| / y</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -124,7 +187,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +240,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -279,17 +356,29 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -659,20 +748,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73ECFD55-E826-4580-9461-72A47B895ECA}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="7" max="7" width="31.21875" customWidth="1"/>
     <col min="8" max="8" width="20.77734375" customWidth="1"/>
     <col min="9" max="9" width="28.109375" customWidth="1"/>
   </cols>
@@ -702,8 +791,8 @@
       <c r="H1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>15</v>
+      <c r="I1" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -737,7 +826,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>3170.9653264765366</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -770,7 +859,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>8192.518606825608</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -803,7 +892,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-2121.9281128253206</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -836,7 +925,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6403.4916316035669</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -869,7 +958,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>3905.9448496181867</v>
       </c>
-      <c r="I6" s="16"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -902,7 +991,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>6493.7214897927261</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -935,7 +1024,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-1051.7252298582025</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -968,7 +1057,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>8948.2747701417975</v>
       </c>
-      <c r="I9" s="16"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1001,7 +1090,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-2908.8420289855203</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1034,7 +1123,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-7064.5121084619095</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1067,7 +1156,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-5901.5121084619095</v>
       </c>
-      <c r="I12" s="16"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1100,7 +1189,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6697.7354682873702</v>
       </c>
-      <c r="I13" s="16"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1133,7 +1222,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-3202.5223468910845</v>
       </c>
-      <c r="I14" s="16"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1166,7 +1255,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6951.9690665420057</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1199,7 +1288,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>1020.24405485428</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1232,7 +1321,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>2554.7768583449943</v>
       </c>
-      <c r="I17" s="16"/>
+      <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -1265,7 +1354,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>12304.10677886862</v>
       </c>
-      <c r="I18" s="16"/>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -1298,7 +1387,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-3287.6800997350947</v>
       </c>
-      <c r="I19" s="16"/>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -1331,7 +1420,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-1756.0202586878731</v>
       </c>
-      <c r="I20" s="16"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -1364,7 +1453,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>1558.4162225338805</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1397,7 +1486,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-801.03049711702624</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -1420,7 +1509,7 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="16"/>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -1436,33 +1525,33 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="15"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="6">
         <f>F23/E23</f>
         <v>9202.2335982546356</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="15"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="5">
         <f>B23-(E26*A23)</f>
         <v>26049.577715443367</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="A30" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
     </row>
     <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
@@ -1471,7 +1560,7 @@
         <v>3</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31" s="9"/>
     </row>
@@ -1486,13 +1575,19 @@
         <v>12</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>2</v>
       </c>
@@ -1507,9 +1602,20 @@
         <f t="shared" ref="D33:D41" si="4">B33-C33</f>
         <v>-929.04491195263836</v>
       </c>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="12">
+        <f>D33*D33</f>
+        <v>863124.44842508552</v>
+      </c>
+      <c r="F33" s="12">
+        <f>(B33-$B$42)^2</f>
+        <v>1686179094.1234567</v>
+      </c>
+      <c r="G33" s="12">
+        <f>IF(D33&lt;0,((D33)*-1)/B33,(D33)/B33)</f>
+        <v>2.1345087006378827E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>3.9</v>
       </c>
@@ -1524,9 +1630,20 @@
         <f>B34-C34</f>
         <v>1279.7112513635584</v>
       </c>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="12">
+        <f t="shared" ref="E34:E41" si="5">D34*D34</f>
+        <v>1637660.8868664845</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" ref="F34:F41" si="6">(B34-$B$42)^2</f>
+        <v>456681648.90123451</v>
+      </c>
+      <c r="G34" s="12">
+        <f t="shared" ref="G34:G41" si="7">IF(D34&lt;0,((D34)*-1)/B34,(D34)/B34)</f>
+        <v>2.0242830386338676E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>4.5</v>
       </c>
@@ -1541,9 +1658,20 @@
         <f t="shared" si="4"/>
         <v>-6348.6289075892273</v>
       </c>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="12">
+        <f t="shared" si="5"/>
+        <v>40305089.006277584</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" si="6"/>
+        <v>551174746.12345672</v>
+      </c>
+      <c r="G35" s="12">
+        <f t="shared" si="7"/>
+        <v>0.10388684373663051</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>5.3</v>
       </c>
@@ -1558,9 +1686,20 @@
         <f t="shared" si="4"/>
         <v>8266.584213807073</v>
       </c>
-      <c r="E36" s="17"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="12">
+        <f t="shared" si="5"/>
+        <v>68336414.563964307</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="6"/>
+        <v>2250333.3456790075</v>
+      </c>
+      <c r="G36" s="12">
+        <f t="shared" si="7"/>
+        <v>9.9491914762746395E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>6</v>
       </c>
@@ -1575,9 +1714,20 @@
         <f t="shared" si="4"/>
         <v>12677.020695028827</v>
       </c>
-      <c r="E37" s="17"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="12">
+        <f t="shared" si="5"/>
+        <v>160706853.70218915</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="6"/>
+        <v>87457825.790123492</v>
+      </c>
+      <c r="G37" s="12">
+        <f t="shared" si="7"/>
+        <v>0.13494805934669818</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>6.8</v>
       </c>
@@ -1592,9 +1742,20 @@
         <f t="shared" si="4"/>
         <v>3113.2338164251123</v>
       </c>
-      <c r="E38" s="17"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="12">
+        <f t="shared" si="5"/>
+        <v>9692224.7957328707</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="6"/>
+        <v>51120911.123456813</v>
+      </c>
+      <c r="G38" s="12">
+        <f t="shared" si="7"/>
+        <v>3.3936142235770482E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>7.1</v>
       </c>
@@ -1609,9 +1770,20 @@
         <f t="shared" si="4"/>
         <v>6887.5637369487231</v>
       </c>
-      <c r="E39" s="17"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="12">
+        <f t="shared" si="5"/>
+        <v>47438534.230531059</v>
+      </c>
+      <c r="F39" s="12">
+        <f t="shared" si="6"/>
+        <v>187276183.90123463</v>
+      </c>
+      <c r="G39" s="12">
+        <f t="shared" si="7"/>
+        <v>7.008602298646345E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>8.6999999999999993</v>
       </c>
@@ -1626,9 +1798,20 @@
         <f t="shared" si="4"/>
         <v>3321.9899797413091</v>
       </c>
-      <c r="E40" s="17"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="12">
+        <f t="shared" si="5"/>
+        <v>11035617.425501663</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" si="6"/>
+        <v>617169128.34567904</v>
+      </c>
+      <c r="G40" s="12">
+        <f t="shared" si="7"/>
+        <v>3.0356937063001427E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>9.5</v>
       </c>
@@ -1643,19 +1826,115 @@
         <f t="shared" si="4"/>
         <v>3498.2031011375948</v>
       </c>
-      <c r="E41" s="17"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C42" s="14" t="s">
-        <v>19</v>
+      <c r="E41" s="12">
+        <f t="shared" si="5"/>
+        <v>12237424.936808685</v>
+      </c>
+      <c r="F41" s="12">
+        <f t="shared" si="6"/>
+        <v>1048521965.234568</v>
+      </c>
+      <c r="G41" s="12">
+        <f t="shared" si="7"/>
+        <v>2.9907095906929141E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3">
+        <f>AVERAGE(B33:B41)</f>
+        <v>84588.111111111109</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3">
+        <f>SUM(E33:E41)</f>
+        <v>352252943.99629688</v>
+      </c>
+      <c r="F42" s="3">
+        <f>SUM(F33:F41)</f>
+        <v>4687831836.8888884</v>
+      </c>
+      <c r="G42" s="3">
+        <f>SUM(G33:G41)</f>
+        <v>0.5442009334309571</v>
+      </c>
+      <c r="H42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18">
+        <f>COUNTA(A33:A41)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E46" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" s="20"/>
+      <c r="G46" s="19">
+        <f>ROUND(1-(E42/F42),4)</f>
+        <v>0.92490000000000006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E47" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="20"/>
+      <c r="G47" s="19">
+        <f>ROUND(E42/C45,3)</f>
+        <v>39139216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E48" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="20"/>
+      <c r="G48" s="19">
+        <f>ROUND((G47)^0.5,3)</f>
+        <v>6256.134</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="22"/>
+      <c r="G49" s="19">
+        <f>ROUND(G42/C45,5)</f>
+        <v>6.0470000000000003E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="I1:I23"/>
-    <mergeCell ref="E32:E41"/>
     <mergeCell ref="A30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
multiple_linear_regession till sir completed
</commit_message>
<xml_diff>
--- a/simple_reg_predict_model.xlsx
+++ b/simple_reg_predict_model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91798\linear_regression_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D93CAA-5501-4615-8BCB-D8FAEAC46A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CEA238-D8DB-48B3-8671-7E85FD386AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D874042-DF0E-4914-8BC4-A047444908B3}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>x</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Error = ei</t>
-  </si>
-  <si>
-    <t>Going to Predict rest of 30% data with repect 70% data of above anlaysis</t>
   </si>
   <si>
     <t xml:space="preserve">  e  = y - ŷ</t>
@@ -178,6 +175,15 @@
       <t>| / y</t>
     </r>
   </si>
+  <si>
+    <t>Predicted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual </t>
+  </si>
+  <si>
+    <t>Going to Predict rest of 30% data with respect 70% data of above anlaysis</t>
+  </si>
 </sst>
 </file>
 
@@ -187,7 +193,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +249,14 @@
     <font>
       <b/>
       <sz val="9.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -339,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -356,17 +370,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -374,11 +379,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -420,6 +438,1010 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Data</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t> Accurancy Check </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$55:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43525</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83088</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93940</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>91738</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98273</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109431</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>116969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A11-4D65-AE30-CEBF79E6ECAC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predicted</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$55:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>44454.044911952638</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61938.288748636442</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67459.628907589227</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74821.415786192927</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81262.979304971173</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88624.766183574888</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91385.436263051277</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106109.01002025869</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>113470.79689886241</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7A11-4D65-AE30-CEBF79E6ECAC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1208319615"/>
+        <c:axId val="1208311295"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1208319615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1208311295"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1208311295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1208319615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{858CB4B8-97A1-4738-B721-DBE9668B48DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -748,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73ECFD55-E826-4580-9461-72A47B895ECA}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,7 +1813,7 @@
       <c r="H1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -826,7 +1848,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>3170.9653264765366</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -859,7 +1881,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>8192.518606825608</v>
       </c>
-      <c r="I3" s="15"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -892,7 +1914,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-2121.9281128253206</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -925,7 +1947,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6403.4916316035669</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -958,7 +1980,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>3905.9448496181867</v>
       </c>
-      <c r="I6" s="15"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -991,7 +2013,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>6493.7214897927261</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1024,7 +2046,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-1051.7252298582025</v>
       </c>
-      <c r="I8" s="15"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1057,7 +2079,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>8948.2747701417975</v>
       </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1090,7 +2112,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-2908.8420289855203</v>
       </c>
-      <c r="I10" s="15"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1123,7 +2145,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-7064.5121084619095</v>
       </c>
-      <c r="I11" s="15"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1156,7 +2178,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-5901.5121084619095</v>
       </c>
-      <c r="I12" s="15"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1189,7 +2211,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6697.7354682873702</v>
       </c>
-      <c r="I13" s="15"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1222,7 +2244,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-3202.5223468910845</v>
       </c>
-      <c r="I14" s="15"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1255,7 +2277,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-6951.9690665420057</v>
       </c>
-      <c r="I15" s="15"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1288,7 +2310,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>1020.24405485428</v>
       </c>
-      <c r="I16" s="15"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1321,7 +2343,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>2554.7768583449943</v>
       </c>
-      <c r="I17" s="15"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -1354,7 +2376,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>12304.10677886862</v>
       </c>
-      <c r="I18" s="15"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -1387,7 +2409,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-3287.6800997350947</v>
       </c>
-      <c r="I19" s="15"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -1420,7 +2442,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-1756.0202586878731</v>
       </c>
-      <c r="I20" s="15"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -1453,7 +2475,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>1558.4162225338805</v>
       </c>
-      <c r="I21" s="15"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1486,7 +2508,7 @@
         <f>Table13[[#This Row],[y]]-Table13[[#This Row],[ ŷ  =  b0  +  b1 * x]]</f>
         <v>-801.03049711702624</v>
       </c>
-      <c r="I22" s="15"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -1509,7 +2531,7 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="15"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -1525,33 +2547,38 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="14"/>
+      <c r="D26" s="21"/>
       <c r="E26" s="6">
         <f>F23/E23</f>
         <v>9202.2335982546356</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="5">
         <f>B23-(E26*A23)</f>
         <v>26049.577715443367</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
+      <c r="I27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
@@ -1562,7 +2589,9 @@
       <c r="D31" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="9"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
@@ -1575,16 +2604,16 @@
         <v>12</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E32" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>20</v>
-      </c>
       <c r="G32" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1845,8 +2874,8 @@
         <f>AVERAGE(B33:B41)</f>
         <v>84588.111111111109</v>
       </c>
-      <c r="C42" s="21" t="s">
-        <v>18</v>
+      <c r="C42" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3">
@@ -1862,85 +2891,166 @@
         <v>0.5442009334309571</v>
       </c>
       <c r="H42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18">
+      <c r="A45" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="18"/>
+      <c r="C45" s="15">
         <f>COUNTA(A33:A41)</f>
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E46" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="19">
+      <c r="E46" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="19"/>
+      <c r="G46" s="16">
         <f>ROUND(1-(E42/F42),4)</f>
         <v>0.92490000000000006</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E47" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="19">
+      <c r="E47" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" s="19"/>
+      <c r="G47" s="16">
         <f>ROUND(E42/C45,3)</f>
         <v>39139216</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E48" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="19">
+      <c r="E48" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="19"/>
+      <c r="G48" s="16">
         <f>ROUND((G47)^0.5,3)</f>
         <v>6256.134</v>
       </c>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E49" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" s="22"/>
-      <c r="G49" s="19">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="20"/>
+      <c r="G49" s="16">
         <f>ROUND(G42/C45,5)</f>
         <v>6.0470000000000003E-2</v>
       </c>
     </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>43525</v>
+      </c>
+      <c r="B55">
+        <v>44454.044911952638</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>63218</v>
+      </c>
+      <c r="B56">
+        <v>61938.288748636442</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>61111</v>
+      </c>
+      <c r="B57">
+        <v>67459.628907589227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>83088</v>
+      </c>
+      <c r="B58">
+        <v>74821.415786192927</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>93940</v>
+      </c>
+      <c r="B59">
+        <v>81262.979304971173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>91738</v>
+      </c>
+      <c r="B60">
+        <v>88624.766183574888</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>98273</v>
+      </c>
+      <c r="B61">
+        <v>91385.436263051277</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>109431</v>
+      </c>
+      <c r="B62">
+        <v>106109.01002025869</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>116969</v>
+      </c>
+      <c r="B63">
+        <v>113470.79689886241</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="I1:I23"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="I1:I23"/>
-    <mergeCell ref="A30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>